<commit_message>
Archivio fine settimana lavorativa
</commit_message>
<xml_diff>
--- a/risultato.xlsx
+++ b/risultato.xlsx
@@ -590,16 +590,16 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>389.4877316876025</v>
+        <v>389.4877318255876</v>
       </c>
       <c r="C5">
-        <v>79.99999999946013</v>
+        <v>79.99999978583787</v>
       </c>
       <c r="D5">
-        <v>38.74576838466137</v>
+        <v>38.74576745149522</v>
       </c>
       <c r="E5">
-        <v>131.762876598775</v>
+        <v>131.7628756641556</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -607,16 +607,16 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>389.4877316876025</v>
+        <v>389.4877318255876</v>
       </c>
       <c r="C6">
-        <v>119.9999999991902</v>
+        <v>119.9999996787568</v>
       </c>
       <c r="D6">
-        <v>58.11865257699204</v>
+        <v>58.11865117724281</v>
       </c>
       <c r="E6">
-        <v>197.6443148981624</v>
+        <v>197.6443134962334</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -624,16 +624,16 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>390.9920209640737</v>
+        <v>390.9920215025131</v>
       </c>
       <c r="C7">
-        <v>39.99999999909859</v>
+        <v>39.99999980483442</v>
       </c>
       <c r="D7">
-        <v>19.37288418642128</v>
+        <v>19.37288266202678</v>
       </c>
       <c r="E7">
-        <v>65.62796831111574</v>
+        <v>65.62796698143455</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -641,16 +641,16 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>390.9920209640737</v>
+        <v>390.9920215025131</v>
       </c>
       <c r="C8">
-        <v>59.99999999864789</v>
+        <v>59.99999970725163</v>
       </c>
       <c r="D8">
-        <v>29.05932627963192</v>
+        <v>29.05932399304016</v>
       </c>
       <c r="E8">
-        <v>98.44195246667358</v>
+        <v>98.44195047215182</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -658,16 +658,16 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>390.3614991762901</v>
+        <v>390.3614997407959</v>
       </c>
       <c r="C9">
-        <v>39.99999999631174</v>
+        <v>39.99999920291975</v>
       </c>
       <c r="D9">
-        <v>-5.52431259848163E-09</v>
+        <v>-1.192816870968727E-06</v>
       </c>
       <c r="E9">
-        <v>59.16057504181678</v>
+        <v>59.16057378286122</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -675,16 +675,16 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>383.6890678123436</v>
+        <v>383.6890695056338</v>
       </c>
       <c r="C10">
-        <v>199.9999999601732</v>
+        <v>199.9999914477247</v>
       </c>
       <c r="D10">
-        <v>96.86442090618738</v>
+        <v>96.86440775791222</v>
       </c>
       <c r="E10">
-        <v>334.3854973905817</v>
+        <v>334.3854757602283</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -692,16 +692,16 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>390.6949328847052</v>
+        <v>390.6949334566526</v>
       </c>
       <c r="C11">
-        <v>149.9999999958534</v>
+        <v>149.9999991032052</v>
       </c>
       <c r="D11">
-        <v>72.64831569855399</v>
+        <v>72.64830986940409</v>
       </c>
       <c r="E11">
-        <v>246.292021617669</v>
+        <v>246.2920163145269</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -728,16 +728,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1492.664422197049</v>
+        <v>1492.664422274971</v>
       </c>
       <c r="C15">
-        <v>199.9999999994575</v>
+        <v>199.9999998133614</v>
       </c>
       <c r="D15">
-        <v>-6.821793476774474E-10</v>
+        <v>-2.324408141021195E-07</v>
       </c>
       <c r="E15">
-        <v>133.9885891465659</v>
+        <v>133.9885890149003</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -745,16 +745,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1492.664422197049</v>
+        <v>1492.664422274971</v>
       </c>
       <c r="C16">
-        <v>199.9999999994575</v>
+        <v>199.9999998133614</v>
       </c>
       <c r="D16">
-        <v>-6.821881015639519E-10</v>
+        <v>-2.324408061440409E-07</v>
       </c>
       <c r="E16">
-        <v>133.9885891465659</v>
+        <v>133.9885890149003</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -762,16 +762,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>390.9920566650646</v>
+        <v>390.9920572034896</v>
       </c>
       <c r="C17">
-        <v>49.99999999560918</v>
+        <v>49.99999905139003</v>
       </c>
       <c r="D17">
-        <v>-6.739451805515273E-09</v>
+        <v>-1.454926377505217E-06</v>
       </c>
       <c r="E17">
-        <v>127.8798357748724</v>
+        <v>127.8798331839534</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -779,16 +779,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>586.0423169453853</v>
+        <v>586.0423178031964</v>
       </c>
       <c r="C18">
-        <v>29.9999999972001</v>
+        <v>29.99999939523494</v>
       </c>
       <c r="D18">
-        <v>-4.068723683303688E-09</v>
+        <v>-8.783536705436746E-07</v>
       </c>
       <c r="E18">
-        <v>51.19084258892413</v>
+        <v>51.19084148677153</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -815,16 +815,16 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>1492.664422197049</v>
+        <v>1492.664422274971</v>
       </c>
       <c r="C22">
-        <v>9.999999999972875</v>
+        <v>9.999999990668071</v>
       </c>
       <c r="D22">
-        <v>-3.410944771076174E-11</v>
+        <v>-1.162204035409786E-08</v>
       </c>
       <c r="E22">
-        <v>6.699429457328292</v>
+        <v>6.699429450745013</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -832,16 +832,16 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>586.4879821496274</v>
+        <v>586.4879829573833</v>
       </c>
       <c r="C23">
-        <v>-9.999999999121835</v>
+        <v>-9.999999810278005</v>
       </c>
       <c r="D23">
-        <v>1.347890815850406E-09</v>
+        <v>2.909852749013453E-07</v>
       </c>
       <c r="E23">
-        <v>17.0506477600259</v>
+        <v>17.05064741453582</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -849,16 +849,16 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>586.04231694616</v>
+        <v>586.0423178039709</v>
       </c>
       <c r="C24">
-        <v>49.9999999953335</v>
+        <v>49.99999899205824</v>
       </c>
       <c r="D24">
-        <v>-6.781202500860673E-09</v>
+        <v>-1.463922787138472E-06</v>
       </c>
       <c r="E24">
-        <v>85.31807098142747</v>
+        <v>85.31806914450645</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -866,16 +866,16 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>602.944588519998</v>
+        <v>602.9445885376979</v>
       </c>
       <c r="C25">
-        <v>99.99999999975211</v>
+        <v>99.99999993000156</v>
       </c>
       <c r="D25">
-        <v>-1.149384729615121E-10</v>
+        <v>-4.56406350792804E-08</v>
       </c>
       <c r="E25">
-        <v>165.852719974177</v>
+        <v>165.8527198536265</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -902,16 +902,16 @@
         <v>24</v>
       </c>
       <c r="B29">
-        <v>746.3322131300656</v>
+        <v>746.3322131690232</v>
       </c>
       <c r="C29">
-        <v>-14.99999999995931</v>
+        <v>-14.99999998600211</v>
       </c>
       <c r="D29">
-        <v>5.116421419870676E-11</v>
+        <v>1.743306001600331E-08</v>
       </c>
       <c r="E29">
-        <v>20.09828831727673</v>
+        <v>20.0982882975266</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -919,16 +919,16 @@
         <v>25</v>
       </c>
       <c r="B30">
-        <v>746.3322131300656</v>
+        <v>746.3322131690232</v>
       </c>
       <c r="C30">
-        <v>-14.99999999995931</v>
+        <v>-14.99999998600211</v>
       </c>
       <c r="D30">
-        <v>5.116421419870676E-11</v>
+        <v>1.743306001600331E-08</v>
       </c>
       <c r="E30">
-        <v>20.09828831727673</v>
+        <v>20.0982882975266</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -936,16 +936,16 @@
         <v>26</v>
       </c>
       <c r="B31">
-        <v>586.4879821496274</v>
+        <v>586.4879829573833</v>
       </c>
       <c r="C31">
-        <v>-29.9999999973655</v>
+        <v>-29.99999943083401</v>
       </c>
       <c r="D31">
-        <v>4.043671765430191E-09</v>
+        <v>8.729558271625138E-07</v>
       </c>
       <c r="E31">
-        <v>51.15194328007768</v>
+        <v>51.15194224360746</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -953,16 +953,16 @@
         <v>27</v>
       </c>
       <c r="B32">
-        <v>586.0423169453853</v>
+        <v>586.0423178031964</v>
       </c>
       <c r="C32">
-        <v>-49.99999999533351</v>
+        <v>-49.99999899205825</v>
       </c>
       <c r="D32">
-        <v>6.781206479899993E-09</v>
+        <v>1.463922786683725E-06</v>
       </c>
       <c r="E32">
-        <v>85.31807098154026</v>
+        <v>85.31806914461924</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -970,16 +970,16 @@
         <v>28</v>
       </c>
       <c r="B33">
-        <v>602.944588519998</v>
+        <v>602.9445885376979</v>
       </c>
       <c r="C33">
-        <v>-39.99999999990084</v>
+        <v>-39.99999997200063</v>
       </c>
       <c r="D33">
-        <v>4.597575298248558E-11</v>
+        <v>1.825625402318565E-08</v>
       </c>
       <c r="E33">
-        <v>66.3410879896708</v>
+        <v>66.3410879414506</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1006,16 +1006,16 @@
         <v>30</v>
       </c>
       <c r="B37">
-        <v>2029.411106802087</v>
+        <v>2029.411106824899</v>
       </c>
       <c r="C37">
-        <v>-139.9999999997744</v>
+        <v>-139.9999999227312</v>
       </c>
       <c r="D37">
-        <v>-90.43106644131224</v>
+        <v>-90.43106628120154</v>
       </c>
       <c r="E37">
-        <v>47.41525486984565</v>
+        <v>47.41525482618598</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1023,16 +1023,16 @@
         <v>31</v>
       </c>
       <c r="B38">
-        <v>2029.411106802087</v>
+        <v>2029.411106824899</v>
       </c>
       <c r="C38">
-        <v>-139.9999999997626</v>
+        <v>-139.999999916552</v>
       </c>
       <c r="D38">
-        <v>-79.34165632090645</v>
+        <v>-79.34165617088203</v>
       </c>
       <c r="E38">
-        <v>45.78024608123027</v>
+        <v>45.78024603907611</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1059,16 +1059,16 @@
         <v>33</v>
       </c>
       <c r="B42">
-        <v>586.04231694616</v>
+        <v>586.0423178039709</v>
       </c>
       <c r="C42">
-        <v>-9.9999999990667</v>
+        <v>-9.999999798411647</v>
       </c>
       <c r="D42">
-        <v>1.356239835104134E-09</v>
+        <v>2.9278455748738E-07</v>
       </c>
       <c r="E42">
-        <v>17.06361419628549</v>
+        <v>17.06361382890129</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1126,28 +1126,28 @@
         <v>44</v>
       </c>
       <c r="B49">
-        <v>19981.41654204961</v>
+        <v>19981.41654245573</v>
       </c>
       <c r="C49">
-        <v>1990.219221646086</v>
+        <v>1990.219221749981</v>
       </c>
       <c r="D49">
-        <v>291.0978468594802</v>
+        <v>291.0978451837209</v>
       </c>
       <c r="E49">
-        <v>290.6670388486574</v>
+        <v>290.6670371781187</v>
       </c>
       <c r="F49">
-        <v>87.95996494553869</v>
+        <v>87.95996414089622</v>
       </c>
       <c r="G49">
-        <v>55.47160846429969</v>
+        <v>55.47160769024637</v>
       </c>
       <c r="H49">
-        <v>8.786685065288221</v>
+        <v>8.786685012030956</v>
       </c>
       <c r="I49">
-        <v>85.84249062297887</v>
+        <v>85.84249010011035</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1155,28 +1155,28 @@
         <v>45</v>
       </c>
       <c r="B50">
-        <v>19981.41654204961</v>
+        <v>19981.41654245573</v>
       </c>
       <c r="C50">
-        <v>1990.219221646086</v>
+        <v>1990.219221749981</v>
       </c>
       <c r="D50">
-        <v>291.0978468594802</v>
+        <v>291.0978451837209</v>
       </c>
       <c r="E50">
-        <v>290.6670388486574</v>
+        <v>290.6670371781187</v>
       </c>
       <c r="F50">
-        <v>87.95996494553869</v>
+        <v>87.95996414089622</v>
       </c>
       <c r="G50">
-        <v>55.47160846429969</v>
+        <v>55.47160769024637</v>
       </c>
       <c r="H50">
-        <v>8.786685065288221</v>
+        <v>8.786685012030956</v>
       </c>
       <c r="I50">
-        <v>85.84249062297887</v>
+        <v>85.84249010011035</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1184,28 +1184,28 @@
         <v>46</v>
       </c>
       <c r="B51">
-        <v>1990.219221646086</v>
+        <v>1990.219221749981</v>
       </c>
       <c r="C51">
-        <v>389.4877316876025</v>
+        <v>389.4877318255876</v>
       </c>
       <c r="D51">
-        <v>201.3340776990581</v>
+        <v>201.3340750800523</v>
       </c>
       <c r="E51">
-        <v>199.9999999934557</v>
+        <v>199.9999974099957</v>
       </c>
       <c r="F51">
-        <v>110.9372365653176</v>
+        <v>110.9372349975222</v>
       </c>
       <c r="G51">
-        <v>96.86442096412833</v>
+        <v>96.8644196053078</v>
       </c>
       <c r="H51">
-        <v>66.68529186365427</v>
+        <v>66.6852909752578</v>
       </c>
       <c r="I51">
-        <v>329.4071914916044</v>
+        <v>329.4071870503547</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1213,28 +1213,28 @@
         <v>47</v>
       </c>
       <c r="B52">
-        <v>19991.44039011284</v>
+        <v>19991.44039087657</v>
       </c>
       <c r="C52">
-        <v>390.9920209640737</v>
+        <v>390.9920215025131</v>
       </c>
       <c r="D52">
-        <v>216.7774911143157</v>
+        <v>216.7774766492043</v>
       </c>
       <c r="E52">
-        <v>215.276000180768</v>
+        <v>215.2759859109946</v>
       </c>
       <c r="F52">
-        <v>114.0867659696281</v>
+        <v>114.0867592606075</v>
       </c>
       <c r="G52">
-        <v>98.96249925331732</v>
+        <v>98.96249369948049</v>
       </c>
       <c r="H52">
-        <v>7.074626028038808</v>
+        <v>7.074625567814823</v>
       </c>
       <c r="I52">
-        <v>349.8691605965054</v>
+        <v>349.8691375430906</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1242,28 +1242,28 @@
         <v>48</v>
       </c>
       <c r="B53">
-        <v>19996.52758352098</v>
+        <v>19996.52758431912</v>
       </c>
       <c r="C53">
-        <v>392.6307249585319</v>
+        <v>392.630725570652</v>
       </c>
       <c r="D53">
-        <v>311.2949197244947</v>
+        <v>311.2948968348108</v>
       </c>
       <c r="E53">
-        <v>309.428287160843</v>
+        <v>309.4282645542194</v>
       </c>
       <c r="F53">
-        <v>143.7099685166015</v>
+        <v>143.7099561083788</v>
       </c>
       <c r="G53">
-        <v>122.7976461084754</v>
+        <v>122.7976353683374</v>
       </c>
       <c r="H53">
-        <v>9.899475463151418</v>
+        <v>9.899474712498384</v>
       </c>
       <c r="I53">
-        <v>489.5309230150622</v>
+        <v>489.5308855231982</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1271,28 +1271,28 @@
         <v>49</v>
       </c>
       <c r="B54">
-        <v>19996.52758352098</v>
+        <v>19996.52758431912</v>
       </c>
       <c r="C54">
-        <v>2009.815281630544</v>
+        <v>2009.81528168955</v>
       </c>
       <c r="D54">
-        <v>-217.7305246758292</v>
+        <v>-217.7305242072229</v>
       </c>
       <c r="E54">
-        <v>-218.0358420321815</v>
+        <v>-218.0358415622719</v>
       </c>
       <c r="F54">
-        <v>-135.0188442199028</v>
+        <v>-135.0188439554549</v>
       </c>
       <c r="G54">
-        <v>-167.2854912898054</v>
+        <v>-167.2854910187111</v>
       </c>
       <c r="H54">
-        <v>7.397041440122383</v>
+        <v>7.397041424311022</v>
       </c>
       <c r="I54">
-        <v>78.94523192939073</v>
+        <v>78.94523177262131</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1331,28 +1331,28 @@
         <v>51</v>
       </c>
       <c r="B58">
-        <v>1990.219221646086</v>
+        <v>1990.219221749981</v>
       </c>
       <c r="C58">
-        <v>1492.664422197049</v>
+        <v>1492.664422274971</v>
       </c>
       <c r="D58">
-        <v>199.9960361355753</v>
+        <v>199.994363128181</v>
       </c>
       <c r="E58">
-        <v>199.9999176402517</v>
+        <v>200.003438768862</v>
       </c>
       <c r="F58">
-        <v>-0.006570675149813724</v>
+        <v>0.006348268891982003</v>
       </c>
       <c r="G58">
-        <v>6.420464727341371E-05</v>
+        <v>0.008778492124223818</v>
       </c>
       <c r="H58">
-        <v>58.01789055403698</v>
+        <v>58.01514330357119</v>
       </c>
       <c r="I58">
-        <v>133.9906155018777</v>
+        <v>133.9902314568286</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1360,25 +1360,25 @@
         <v>52</v>
       </c>
       <c r="B59">
-        <v>1990.219221646086</v>
+        <v>1990.219221749981</v>
       </c>
       <c r="C59">
-        <v>1492.664422197049</v>
+        <v>1492.664422274971</v>
       </c>
       <c r="D59">
-        <v>179.9964516690939</v>
+        <v>179.9941523191701</v>
       </c>
       <c r="E59">
-        <v>180.0022976645012</v>
+        <v>180.0022935533734</v>
       </c>
       <c r="F59">
-        <v>-0.0009280973862200882</v>
+        <v>0.002939366966476428</v>
       </c>
       <c r="G59">
-        <v>0.004866406045566578</v>
+        <v>0.004415428849018781</v>
       </c>
       <c r="H59">
-        <v>52.21888096713357</v>
+        <v>52.21562209227531</v>
       </c>
       <c r="I59">
         <v>120.5931289233772</v>
@@ -1389,28 +1389,28 @@
         <v>53</v>
       </c>
       <c r="B60">
-        <v>390.9920209640737</v>
+        <v>390.9920215025131</v>
       </c>
       <c r="C60">
-        <v>586.4879821496274</v>
+        <v>586.4879829573833</v>
       </c>
       <c r="D60">
-        <v>75.21722211260767</v>
+        <v>75.2182949705508</v>
       </c>
       <c r="E60">
-        <v>75.21938110307406</v>
+        <v>75.21943558418545</v>
       </c>
       <c r="F60">
-        <v>50.52570625272507</v>
+        <v>50.50333516189703</v>
       </c>
       <c r="G60">
-        <v>50.50994964744115</v>
+        <v>50.47960675645903</v>
       </c>
       <c r="H60">
-        <v>133.8318565226998</v>
+        <v>133.8033844980201</v>
       </c>
       <c r="I60">
-        <v>154.4858742432156</v>
+        <v>154.404914706582</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1418,28 +1418,28 @@
         <v>54</v>
       </c>
       <c r="B61">
-        <v>390.6949328847052</v>
+        <v>390.6949334566526</v>
       </c>
       <c r="C61">
-        <v>586.04231694616</v>
+        <v>586.0423178039709</v>
       </c>
       <c r="D61">
-        <v>-25.16396405201149</v>
+        <v>-25.15875725152281</v>
       </c>
       <c r="E61">
-        <v>-25.16061800412298</v>
+        <v>-25.15971686606806</v>
       </c>
       <c r="F61">
-        <v>-50.44830384367348</v>
+        <v>-50.44664287785054</v>
       </c>
       <c r="G61">
-        <v>-50.44674228998612</v>
+        <v>-50.44165817080625</v>
       </c>
       <c r="H61">
-        <v>83.30073078471507</v>
+        <v>83.29330985690835</v>
       </c>
       <c r="I61">
-        <v>96.18933419101717</v>
+        <v>96.17403605037291</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1447,28 +1447,28 @@
         <v>55</v>
       </c>
       <c r="B62">
-        <v>390.6949328847052</v>
+        <v>390.6949334566526</v>
       </c>
       <c r="C62">
-        <v>586.0423169453853</v>
+        <v>586.0423178031964</v>
       </c>
       <c r="D62">
-        <v>-20.00082902549808</v>
+        <v>-20.0014096484914</v>
       </c>
       <c r="E62">
-        <v>-20.00094968750714</v>
+        <v>-20.00245079530523</v>
       </c>
       <c r="F62">
-        <v>-0.00101769096749581</v>
+        <v>-0.002231392821311033</v>
       </c>
       <c r="G62">
-        <v>-0.001100416456200662</v>
+        <v>0.0007522937014116734</v>
       </c>
       <c r="H62">
-        <v>29.55430647553754</v>
+        <v>29.55968424833608</v>
       </c>
       <c r="I62">
-        <v>34.12960616663842</v>
+        <v>34.12833818153045</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -1476,28 +1476,28 @@
         <v>56</v>
       </c>
       <c r="B63">
-        <v>2009.815281630544</v>
+        <v>2009.81528168955</v>
       </c>
       <c r="C63">
-        <v>602.944588519998</v>
+        <v>602.9445885376979</v>
       </c>
       <c r="D63">
-        <v>59.99975599508041</v>
+        <v>59.99987326924993</v>
       </c>
       <c r="E63">
-        <v>59.99940231954785</v>
+        <v>60.00021625807812</v>
       </c>
       <c r="F63">
-        <v>-0.007128145070463632</v>
+        <v>-0.004836555941451451</v>
       </c>
       <c r="G63">
-        <v>-0.002579338811256335</v>
+        <v>-0.001124051604098369</v>
       </c>
       <c r="H63">
-        <v>17.23613937151823</v>
+        <v>17.23624520930266</v>
       </c>
       <c r="I63">
-        <v>99.50931049281699</v>
+        <v>99.51515143735945</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -1536,28 +1536,28 @@
         <v>58</v>
       </c>
       <c r="B67">
-        <v>1492.664422197049</v>
+        <v>1492.664422274971</v>
       </c>
       <c r="C67">
-        <v>746.3322131300656</v>
+        <v>746.3322131690232</v>
       </c>
       <c r="D67">
-        <v>-30.00023507626074</v>
+        <v>-30.00020964141612</v>
       </c>
       <c r="E67">
-        <v>-29.99996713068388</v>
+        <v>-30.00009391353698</v>
       </c>
       <c r="F67">
-        <v>-0.001040022058916307</v>
+        <v>-0.001134635891084315</v>
       </c>
       <c r="G67">
-        <v>-3.649684199012881E-05</v>
+        <v>1.726125258277022E-05</v>
       </c>
       <c r="H67">
-        <v>20.09839065366581</v>
+        <v>20.0981825890309</v>
       </c>
       <c r="I67">
-        <v>40.19655541232466</v>
+        <v>40.19670076572509</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -1565,25 +1565,25 @@
         <v>59</v>
       </c>
       <c r="B68">
-        <v>586.4879821496274</v>
+        <v>586.4879829573833</v>
       </c>
       <c r="C68">
-        <v>390.9920566650646</v>
+        <v>390.9920572034896</v>
       </c>
       <c r="D68">
-        <v>49.99957539238897</v>
+        <v>49.99969066422425</v>
       </c>
       <c r="E68">
-        <v>50.00242982628541</v>
+        <v>50.0022101445969</v>
       </c>
       <c r="F68">
-        <v>-0.005350242137555597</v>
+        <v>-0.006257545078988984</v>
       </c>
       <c r="G68">
-        <v>0.002233401586914965</v>
+        <v>0.000475867418026269</v>
       </c>
       <c r="H68">
-        <v>85.25417708625902</v>
+        <v>85.25248643040224</v>
       </c>
       <c r="I68">
         <v>127.8892547627229</v>
@@ -1625,28 +1625,28 @@
         <v>61</v>
       </c>
       <c r="B72">
-        <v>19997.75723932969</v>
+        <v>19997.75723962632</v>
       </c>
       <c r="C72">
-        <v>19981.41654204961</v>
+        <v>19981.41654245573</v>
       </c>
       <c r="D72">
-        <v>582.6315290937978</v>
+        <v>582.6315257369653</v>
       </c>
       <c r="E72">
-        <v>582.1956937189696</v>
+        <v>582.1956903674263</v>
       </c>
       <c r="F72">
-        <v>66.99862559929757</v>
+        <v>66.998623982542</v>
       </c>
       <c r="G72">
-        <v>175.9199298911245</v>
+        <v>175.9199282817469</v>
       </c>
       <c r="H72">
-        <v>16.93186011004118</v>
+        <v>16.93186000817659</v>
       </c>
       <c r="I72">
-        <v>17.57337013057525</v>
+        <v>17.57337002406266</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -1654,28 +1654,28 @@
         <v>62</v>
       </c>
       <c r="B73">
-        <v>19997.75723932969</v>
+        <v>19997.75723962632</v>
       </c>
       <c r="C73">
-        <v>19991.44039011284</v>
+        <v>19991.44039087657</v>
       </c>
       <c r="D73">
-        <v>216.8396951904256</v>
+        <v>216.8396807166607</v>
       </c>
       <c r="E73">
-        <v>216.7774911143611</v>
+        <v>216.7774766492678</v>
       </c>
       <c r="F73">
-        <v>4.860098120989678</v>
+        <v>4.860091400329917</v>
       </c>
       <c r="G73">
-        <v>114.0867659696952</v>
+        <v>114.0867592606651</v>
       </c>
       <c r="H73">
-        <v>6.261888530483725</v>
+        <v>6.261888108244006</v>
       </c>
       <c r="I73">
-        <v>7.074626028039121</v>
+        <v>7.074625567814897</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -1683,28 +1683,28 @@
         <v>63</v>
       </c>
       <c r="B74">
-        <v>390.9920209640737</v>
+        <v>390.9920215025131</v>
       </c>
       <c r="C74">
-        <v>390.3614991762901</v>
+        <v>390.3614997407959</v>
       </c>
       <c r="D74">
-        <v>40.06457443846671</v>
+        <v>40.06457288426982</v>
       </c>
       <c r="E74">
-        <v>39.99999999279861</v>
+        <v>39.99999844378982</v>
       </c>
       <c r="F74">
-        <v>0.05249954906050687</v>
+        <v>0.05249948831484329</v>
       </c>
       <c r="G74">
-        <v>-2.631501843097795E-10</v>
+        <v>-5.679085609244794E-08</v>
       </c>
       <c r="H74">
-        <v>59.16057503661947</v>
+        <v>59.16057266012713</v>
       </c>
       <c r="I74">
-        <v>59.16057503661947</v>
+        <v>59.16057266012713</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -1712,28 +1712,28 @@
         <v>64</v>
       </c>
       <c r="B75">
-        <v>19997.75723932969</v>
+        <v>19997.75723962632</v>
       </c>
       <c r="C75">
-        <v>19996.52758352098</v>
+        <v>19996.52758431912</v>
       </c>
       <c r="D75">
-        <v>93.57220722080152</v>
+        <v>93.57218479693776</v>
       </c>
       <c r="E75">
-        <v>93.56439504867653</v>
+        <v>93.56437262763318</v>
       </c>
       <c r="F75">
-        <v>-64.16776264917112</v>
+        <v>-64.1677747988345</v>
       </c>
       <c r="G75">
-        <v>8.691124296658179</v>
+        <v>8.691112152841136</v>
       </c>
       <c r="H75">
-        <v>3.275636813230302</v>
+        <v>3.275636477606379</v>
       </c>
       <c r="I75">
-        <v>2.713101582355106</v>
+        <v>2.713100905171892</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -1741,28 +1741,28 @@
         <v>65</v>
       </c>
       <c r="B76">
-        <v>392.6307249585319</v>
+        <v>392.630725570652</v>
       </c>
       <c r="C76">
-        <v>383.6890678123436</v>
+        <v>383.6890695056338</v>
       </c>
       <c r="D76">
-        <v>204.1259221858112</v>
+        <v>204.1258983340154</v>
       </c>
       <c r="E76">
-        <v>199.9999998931405</v>
+        <v>199.9999770326304</v>
       </c>
       <c r="F76">
-        <v>100.2188292804771</v>
+        <v>100.2188166816432</v>
       </c>
       <c r="G76">
-        <v>96.86442091245212</v>
+        <v>96.86440911954156</v>
       </c>
       <c r="H76">
-        <v>334.3854973038738</v>
+        <v>334.3854571290636</v>
       </c>
       <c r="I76">
-        <v>334.3854973038738</v>
+        <v>334.3854571290636</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -1770,28 +1770,28 @@
         <v>66</v>
       </c>
       <c r="B77">
-        <v>392.6307249585319</v>
+        <v>392.630725570652</v>
       </c>
       <c r="C77">
-        <v>390.6949328847052</v>
+        <v>390.6949334566526</v>
       </c>
       <c r="D77">
-        <v>105.3023649750302</v>
+        <v>105.3023662202068</v>
       </c>
       <c r="E77">
-        <v>104.8396600406415</v>
+        <v>104.8396612734503</v>
       </c>
       <c r="F77">
-        <v>22.57881682799869</v>
+        <v>22.57881868669629</v>
       </c>
       <c r="G77">
-        <v>22.2026339545119</v>
+        <v>22.20263580315441</v>
       </c>
       <c r="H77">
-        <v>158.3698419937845</v>
+        <v>158.3698441106598</v>
       </c>
       <c r="I77">
-        <v>158.3698419937845</v>
+        <v>158.3698441106598</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -1799,28 +1799,28 @@
         <v>67</v>
       </c>
       <c r="B78">
-        <v>2009.815281630544</v>
+        <v>2009.81528168955</v>
       </c>
       <c r="C78">
-        <v>2029.411106802087</v>
+        <v>2029.411106824899</v>
       </c>
       <c r="D78">
-        <v>-278.0358420319743</v>
+        <v>-278.0358415195804</v>
       </c>
       <c r="E78">
-        <v>-279.9999999986898</v>
+        <v>-279.9999994790002</v>
       </c>
       <c r="F78">
-        <v>-167.2788564083448</v>
+        <v>-167.278856110206</v>
       </c>
       <c r="G78">
-        <v>-169.7727227621275</v>
+        <v>-169.7727224533312</v>
       </c>
       <c r="H78">
-        <v>93.21135927814241</v>
+        <v>93.21135910512457</v>
       </c>
       <c r="I78">
-        <v>93.1564362528453</v>
+        <v>93.15643607982241</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -1859,28 +1859,28 @@
         <v>69</v>
       </c>
       <c r="B82">
-        <v>586.04231694616</v>
+        <v>586.0423178039709</v>
       </c>
       <c r="C82">
-        <v>586.4879821496274</v>
+        <v>586.4879829573833</v>
       </c>
       <c r="D82">
-        <v>-65.16278586019601</v>
+        <v>-65.16277787202941</v>
       </c>
       <c r="E82">
-        <v>-65.21142576404947</v>
+        <v>-65.21141776491942</v>
       </c>
       <c r="F82">
-        <v>-50.44338788318483</v>
+        <v>-50.44338323266573</v>
       </c>
       <c r="G82">
-        <v>-50.48292517790316</v>
+        <v>-50.4829205184717</v>
       </c>
       <c r="H82">
-        <v>140.6096476204726</v>
+        <v>140.6096317784082</v>
       </c>
       <c r="I82">
-        <v>140.6096399542044</v>
+        <v>140.609624112097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creata la lettura delle righe di dss. Provo a convertire il metodo con tale approccio
</commit_message>
<xml_diff>
--- a/risultato.xlsx
+++ b/risultato.xlsx
@@ -590,16 +590,16 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>389.4877318255876</v>
+        <v>390.0770000151745</v>
       </c>
       <c r="C5">
-        <v>79.99999978583787</v>
+        <v>80</v>
       </c>
       <c r="D5">
-        <v>38.74576745149522</v>
+        <v>38.7457683870282</v>
       </c>
       <c r="E5">
-        <v>131.7628756641556</v>
+        <v>131.5638295156349</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -607,16 +607,16 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>389.4877318255876</v>
+        <v>390.0770000151745</v>
       </c>
       <c r="C6">
-        <v>119.9999996787568</v>
+        <v>120</v>
       </c>
       <c r="D6">
-        <v>58.11865117724281</v>
+        <v>58.1186525805423</v>
       </c>
       <c r="E6">
-        <v>197.6443134962334</v>
+        <v>197.3457442734524</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -624,16 +624,16 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>390.9920215025131</v>
+        <v>391.0119755478833</v>
       </c>
       <c r="C7">
-        <v>39.99999980483442</v>
+        <v>39.99999999999793</v>
       </c>
       <c r="D7">
-        <v>19.37288266202678</v>
+        <v>19.37288419351511</v>
       </c>
       <c r="E7">
-        <v>65.62796698143455</v>
+        <v>65.62461911308367</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -641,16 +641,16 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>390.9920215025131</v>
+        <v>391.0119755478833</v>
       </c>
       <c r="C8">
-        <v>59.99999970725163</v>
+        <v>59.99999999999687</v>
       </c>
       <c r="D8">
-        <v>29.05932399304016</v>
+        <v>29.05932629027266</v>
       </c>
       <c r="E8">
-        <v>98.44195047215182</v>
+        <v>98.4369286696255</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -658,16 +658,16 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>390.3614997407959</v>
+        <v>390.3814865225988</v>
       </c>
       <c r="C9">
-        <v>39.99999920291975</v>
+        <v>39.99999999999871</v>
       </c>
       <c r="D9">
-        <v>-1.192816870968727E-06</v>
+        <v>1.636578872421524E-12</v>
       </c>
       <c r="E9">
-        <v>59.16057378286122</v>
+        <v>59.15754605399023</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -675,16 +675,16 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>383.6890695056338</v>
+        <v>383.7093736109052</v>
       </c>
       <c r="C10">
-        <v>199.9999914477247</v>
+        <v>200</v>
       </c>
       <c r="D10">
-        <v>96.86440775791222</v>
+        <v>96.86442096757048</v>
       </c>
       <c r="E10">
-        <v>334.3854757602283</v>
+        <v>334.3678018927355</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -692,16 +692,16 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>390.6949334566526</v>
+        <v>390.7147973406008</v>
       </c>
       <c r="C11">
-        <v>149.9999991032052</v>
+        <v>150</v>
       </c>
       <c r="D11">
-        <v>72.64830986940409</v>
+        <v>72.64831572567788</v>
       </c>
       <c r="E11">
-        <v>246.2920163145269</v>
+        <v>246.2794998292696</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -728,16 +728,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1492.664422274971</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>199.9999998133614</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>-2.324408141021195E-07</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>133.9885890149003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -745,16 +745,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1492.664422274971</v>
+        <v>1354.966545725536</v>
       </c>
       <c r="C16">
-        <v>199.9999998133614</v>
+        <v>20.01755005170917</v>
       </c>
       <c r="D16">
-        <v>-2.324408061440409E-07</v>
+        <v>-0.0001865144429667751</v>
       </c>
       <c r="E16">
-        <v>133.9885890149003</v>
+        <v>14.77346370268729</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -762,16 +762,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>390.9920572034896</v>
+        <v>391.0120092064996</v>
       </c>
       <c r="C17">
-        <v>49.99999905139003</v>
+        <v>49.9999999999984</v>
       </c>
       <c r="D17">
-        <v>-1.454926377505217E-06</v>
+        <v>2.041815605480224E-12</v>
       </c>
       <c r="E17">
-        <v>127.8798331839534</v>
+        <v>127.8733103401842</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -779,16 +779,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>586.0423178031964</v>
+        <v>586.0722512117063</v>
       </c>
       <c r="C18">
-        <v>29.99999939523494</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>-8.783536705436746E-07</v>
+        <v>7.958078640513122E-16</v>
       </c>
       <c r="E18">
-        <v>51.19084148677153</v>
+        <v>51.18822796673089</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -815,16 +815,16 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>1492.664422274971</v>
+        <v>1354.966545725536</v>
       </c>
       <c r="C22">
-        <v>9.999999990668071</v>
+        <v>81.52554998775024</v>
       </c>
       <c r="D22">
-        <v>-1.162204035409786E-08</v>
+        <v>-0.0007596180594018734</v>
       </c>
       <c r="E22">
-        <v>6.699429450745013</v>
+        <v>60.16794076037835</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -832,16 +832,16 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>586.4879829573833</v>
+        <v>586.5178881786698</v>
       </c>
       <c r="C23">
-        <v>-9.999999810278005</v>
+        <v>-9.99999999999968</v>
       </c>
       <c r="D23">
-        <v>2.909852749013453E-07</v>
+        <v>-4.078231086168671E-13</v>
       </c>
       <c r="E23">
-        <v>17.05064741453582</v>
+        <v>17.0497783640551</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -849,16 +849,16 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>586.0423178039709</v>
+        <v>586.0722512124808</v>
       </c>
       <c r="C24">
-        <v>49.99999899205824</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>-1.463922787138472E-06</v>
+        <v>1.818989403545857E-15</v>
       </c>
       <c r="E24">
-        <v>85.31806914450645</v>
+        <v>85.31371327777207</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -866,16 +866,16 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>602.9445885376979</v>
+        <v>602.9735305280847</v>
       </c>
       <c r="C25">
-        <v>99.99999993000156</v>
+        <v>100.0000000000006</v>
       </c>
       <c r="D25">
-        <v>-4.56406350792804E-08</v>
+        <v>1.33240973809734E-13</v>
       </c>
       <c r="E25">
-        <v>165.8527198536265</v>
+        <v>165.8447592424503</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -902,16 +902,16 @@
         <v>24</v>
       </c>
       <c r="B29">
-        <v>746.3322131690232</v>
+        <v>677.4830753872644</v>
       </c>
       <c r="C29">
-        <v>-14.99999998600211</v>
+        <v>-122.2883249816272</v>
       </c>
       <c r="D29">
-        <v>1.743306001600331E-08</v>
+        <v>0.001139429630412053</v>
       </c>
       <c r="E29">
-        <v>20.0982882975266</v>
+        <v>180.5038272445742</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -919,16 +919,16 @@
         <v>25</v>
       </c>
       <c r="B30">
-        <v>746.3322131690232</v>
+        <v>677.4830753872644</v>
       </c>
       <c r="C30">
-        <v>-14.99999998600211</v>
+        <v>-122.2883249816272</v>
       </c>
       <c r="D30">
-        <v>1.743306001600331E-08</v>
+        <v>0.001139429630412053</v>
       </c>
       <c r="E30">
-        <v>20.0982882975266</v>
+        <v>180.5038272445742</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -936,16 +936,16 @@
         <v>26</v>
       </c>
       <c r="B31">
-        <v>586.4879829573833</v>
+        <v>586.5178881786698</v>
       </c>
       <c r="C31">
-        <v>-29.99999943083401</v>
+        <v>-29.99999999999904</v>
       </c>
       <c r="D31">
-        <v>8.729558271625138E-07</v>
+        <v>-1.224861989612691E-12</v>
       </c>
       <c r="E31">
-        <v>51.15194224360746</v>
+        <v>51.1493350921653</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -953,16 +953,16 @@
         <v>27</v>
       </c>
       <c r="B32">
-        <v>586.0423178031964</v>
+        <v>586.0722512117063</v>
       </c>
       <c r="C32">
-        <v>-49.99999899205825</v>
+        <v>-49.99999999999999</v>
       </c>
       <c r="D32">
-        <v>1.463922786683725E-06</v>
+        <v>-8.526512829121202E-16</v>
       </c>
       <c r="E32">
-        <v>85.31806914461924</v>
+        <v>85.31371327788482</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -970,16 +970,16 @@
         <v>28</v>
       </c>
       <c r="B33">
-        <v>602.9445885376979</v>
+        <v>602.9735305280847</v>
       </c>
       <c r="C33">
-        <v>-39.99999997200063</v>
+        <v>-40.00000000000024</v>
       </c>
       <c r="D33">
-        <v>1.825625402318565E-08</v>
+        <v>-5.312017492542508E-14</v>
       </c>
       <c r="E33">
-        <v>66.3410879414506</v>
+        <v>66.33790369698012</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1006,16 +1006,16 @@
         <v>30</v>
       </c>
       <c r="B37">
-        <v>2029.411106824899</v>
+        <v>2029.50666434999</v>
       </c>
       <c r="C37">
-        <v>-139.9999999227312</v>
+        <v>-140.0000000000007</v>
       </c>
       <c r="D37">
-        <v>-90.43106628120154</v>
+        <v>-90.43106644167099</v>
       </c>
       <c r="E37">
-        <v>47.41525482618598</v>
+        <v>47.41302236410993</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1023,16 +1023,16 @@
         <v>31</v>
       </c>
       <c r="B38">
-        <v>2029.411106824899</v>
+        <v>2029.50666434999</v>
       </c>
       <c r="C38">
-        <v>-139.999999916552</v>
+        <v>-140.0000000000007</v>
       </c>
       <c r="D38">
-        <v>-79.34165617088203</v>
+        <v>-79.34165632123961</v>
       </c>
       <c r="E38">
-        <v>45.78024603907611</v>
+        <v>45.77809055845096</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1059,16 +1059,16 @@
         <v>33</v>
       </c>
       <c r="B42">
-        <v>586.0423178039709</v>
+        <v>586.0722512124808</v>
       </c>
       <c r="C42">
-        <v>-9.999999798411647</v>
+        <v>-10</v>
       </c>
       <c r="D42">
-        <v>2.9278455748738E-07</v>
+        <v>2.1316282072803E-16</v>
       </c>
       <c r="E42">
-        <v>17.06361382890129</v>
+        <v>17.06274265555441</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1126,28 +1126,28 @@
         <v>44</v>
       </c>
       <c r="B49">
-        <v>19981.41654245573</v>
+        <v>19991.83895448359</v>
       </c>
       <c r="C49">
-        <v>1990.219221749981</v>
+        <v>1993.104211821479</v>
       </c>
       <c r="D49">
-        <v>291.0978451837209</v>
+        <v>100.746558779756</v>
       </c>
       <c r="E49">
-        <v>290.6670371781187</v>
+        <v>100.6650747866874</v>
       </c>
       <c r="F49">
-        <v>87.95996414089622</v>
+        <v>85.7868672670006</v>
       </c>
       <c r="G49">
-        <v>55.47160769024637</v>
+        <v>55.46602179722338</v>
       </c>
       <c r="H49">
-        <v>8.786685012030956</v>
+        <v>3.821382138521454</v>
       </c>
       <c r="I49">
-        <v>85.84249010011035</v>
+        <v>33.29352170595222</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1155,28 +1155,28 @@
         <v>45</v>
       </c>
       <c r="B50">
-        <v>19981.41654245573</v>
+        <v>19991.83895448359</v>
       </c>
       <c r="C50">
-        <v>1990.219221749981</v>
+        <v>1993.104211821479</v>
       </c>
       <c r="D50">
-        <v>291.0978451837209</v>
+        <v>100.746558779756</v>
       </c>
       <c r="E50">
-        <v>290.6670371781187</v>
+        <v>100.6650747866874</v>
       </c>
       <c r="F50">
-        <v>87.95996414089622</v>
+        <v>85.7868672670006</v>
       </c>
       <c r="G50">
-        <v>55.47160769024637</v>
+        <v>55.46602179722338</v>
       </c>
       <c r="H50">
-        <v>8.786685012030956</v>
+        <v>3.821382138521454</v>
       </c>
       <c r="I50">
-        <v>85.84249010011035</v>
+        <v>33.29352170595222</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1184,28 +1184,28 @@
         <v>46</v>
       </c>
       <c r="B51">
-        <v>1990.219221749981</v>
+        <v>1993.104211821479</v>
       </c>
       <c r="C51">
-        <v>389.4877318255876</v>
+        <v>390.0770000151745</v>
       </c>
       <c r="D51">
-        <v>201.3340750800523</v>
+        <v>201.3301495654292</v>
       </c>
       <c r="E51">
-        <v>199.9999974099957</v>
+        <v>200.0000000000006</v>
       </c>
       <c r="F51">
-        <v>110.9372349975222</v>
+        <v>110.9320435944472</v>
       </c>
       <c r="G51">
-        <v>96.8644196053078</v>
+        <v>96.86442096757094</v>
       </c>
       <c r="H51">
-        <v>66.6852909752578</v>
+        <v>66.58704340988417</v>
       </c>
       <c r="I51">
-        <v>329.4071870503547</v>
+        <v>328.9095737890887</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1213,28 +1213,28 @@
         <v>47</v>
       </c>
       <c r="B52">
-        <v>19991.44039087657</v>
+        <v>19992.41183508806</v>
       </c>
       <c r="C52">
-        <v>390.9920215025131</v>
+        <v>391.0119755478833</v>
       </c>
       <c r="D52">
-        <v>216.7774766492043</v>
+        <v>216.776119104398</v>
       </c>
       <c r="E52">
-        <v>215.2759859109946</v>
+        <v>215.2747887781741</v>
       </c>
       <c r="F52">
-        <v>114.0867592606075</v>
+        <v>114.0867981039403</v>
       </c>
       <c r="G52">
-        <v>98.96249369948049</v>
+        <v>98.96287412116075</v>
       </c>
       <c r="H52">
-        <v>7.074625567814823</v>
+        <v>7.074249419306123</v>
       </c>
       <c r="I52">
-        <v>349.8691375430906</v>
+        <v>349.8477544884278</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1242,28 +1242,28 @@
         <v>48</v>
       </c>
       <c r="B53">
-        <v>19996.52758431912</v>
+        <v>19997.49870920183</v>
       </c>
       <c r="C53">
-        <v>392.630725570652</v>
+        <v>392.6505533150195</v>
       </c>
       <c r="D53">
-        <v>311.2948968348108</v>
+        <v>311.293282072608</v>
       </c>
       <c r="E53">
-        <v>309.4282645542194</v>
+        <v>309.4268461673401</v>
       </c>
       <c r="F53">
-        <v>143.7099561083788</v>
+        <v>143.7101467674327</v>
       </c>
       <c r="G53">
-        <v>122.7976353683374</v>
+        <v>122.7980265354749</v>
       </c>
       <c r="H53">
-        <v>9.899474712498384</v>
+        <v>9.898946359505542</v>
       </c>
       <c r="I53">
-        <v>489.5308855231982</v>
+        <v>489.5050681257725</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1271,28 +1271,28 @@
         <v>49</v>
       </c>
       <c r="B54">
-        <v>19996.52758431912</v>
+        <v>19997.49870920183</v>
       </c>
       <c r="C54">
-        <v>2009.81528168955</v>
+        <v>2009.911759163232</v>
       </c>
       <c r="D54">
-        <v>-217.7305242072229</v>
+        <v>-217.7307417301425</v>
       </c>
       <c r="E54">
-        <v>-218.0358415622719</v>
+        <v>-218.036026866227</v>
       </c>
       <c r="F54">
-        <v>-135.0188439554549</v>
+        <v>-135.0164491780118</v>
       </c>
       <c r="G54">
-        <v>-167.2854910187111</v>
+        <v>-167.2857969090567</v>
       </c>
       <c r="H54">
-        <v>7.397041424311022</v>
+        <v>7.39665112388319</v>
       </c>
       <c r="I54">
-        <v>78.94523177262131</v>
+        <v>78.94153801240478</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1331,28 +1331,28 @@
         <v>51</v>
       </c>
       <c r="B58">
-        <v>1990.219221749981</v>
+        <v>1993.104211821479</v>
       </c>
       <c r="C58">
-        <v>1492.664422274971</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>199.994363128181</v>
+        <v>3.972464406649234E-09</v>
       </c>
       <c r="E58">
-        <v>200.003438768862</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>0.006348268891982003</v>
+        <v>1.058791184067875E-25</v>
       </c>
       <c r="G58">
-        <v>0.008778492124223818</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>58.01514330357119</v>
+        <v>1.150719253218108E-09</v>
       </c>
       <c r="I58">
-        <v>133.9902314568286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1360,28 +1360,28 @@
         <v>52</v>
       </c>
       <c r="B59">
-        <v>1990.219221749981</v>
+        <v>1993.104211821479</v>
       </c>
       <c r="C59">
-        <v>1492.664422274971</v>
+        <v>1354.966545725536</v>
       </c>
       <c r="D59">
-        <v>179.9941523191701</v>
+        <v>3.972464406649234E-09</v>
       </c>
       <c r="E59">
-        <v>180.0022935533734</v>
+        <v>-1.835934499704411E-09</v>
       </c>
       <c r="F59">
-        <v>0.002939366966476428</v>
+        <v>1.058791184067875E-25</v>
       </c>
       <c r="G59">
-        <v>0.004415428849018781</v>
+        <v>-5.293955920339377E-26</v>
       </c>
       <c r="H59">
-        <v>52.21562209227531</v>
+        <v>1.150719253218108E-09</v>
       </c>
       <c r="I59">
-        <v>120.5931289233772</v>
+        <v>1.354966545725537E-09</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1389,28 +1389,28 @@
         <v>53</v>
       </c>
       <c r="B60">
-        <v>390.9920215025131</v>
+        <v>391.0119755478833</v>
       </c>
       <c r="C60">
-        <v>586.4879829573833</v>
+        <v>586.5178881786698</v>
       </c>
       <c r="D60">
-        <v>75.2182949705508</v>
+        <v>75.220734335877</v>
       </c>
       <c r="E60">
-        <v>75.21943558418545</v>
+        <v>75.19441776525738</v>
       </c>
       <c r="F60">
-        <v>50.50333516189703</v>
+        <v>50.46965844039665</v>
       </c>
       <c r="G60">
-        <v>50.47960675645903</v>
+        <v>50.44431608087888</v>
       </c>
       <c r="H60">
-        <v>133.8033844980201</v>
+        <v>133.7864627940851</v>
       </c>
       <c r="I60">
-        <v>154.404914706582</v>
+        <v>154.3816362692046</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1418,28 +1418,28 @@
         <v>54</v>
       </c>
       <c r="B61">
-        <v>390.6949334566526</v>
+        <v>390.7147973406008</v>
       </c>
       <c r="C61">
-        <v>586.0423178039709</v>
+        <v>586.0722512124808</v>
       </c>
       <c r="D61">
-        <v>-25.15875725152281</v>
+        <v>-25.16261565403326</v>
       </c>
       <c r="E61">
-        <v>-25.15971686606806</v>
+        <v>-25.16461410261487</v>
       </c>
       <c r="F61">
-        <v>-50.44664287785054</v>
+        <v>-50.44621212878806</v>
       </c>
       <c r="G61">
-        <v>-50.44165817080625</v>
+        <v>-50.44426516573817</v>
       </c>
       <c r="H61">
-        <v>83.29330985690835</v>
+        <v>83.28957374873137</v>
       </c>
       <c r="I61">
-        <v>96.17403605037291</v>
+        <v>96.17006688312448</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1447,28 +1447,28 @@
         <v>55</v>
       </c>
       <c r="B62">
-        <v>390.6949334566526</v>
+        <v>390.7147973406008</v>
       </c>
       <c r="C62">
-        <v>586.0423178031964</v>
+        <v>586.0722512117063</v>
       </c>
       <c r="D62">
-        <v>-20.0014096484914</v>
+        <v>-19.99964045259352</v>
       </c>
       <c r="E62">
-        <v>-20.00245079530523</v>
+        <v>-20.0011205116319</v>
       </c>
       <c r="F62">
-        <v>-0.002231392821311033</v>
+        <v>-0.004219132152220368</v>
       </c>
       <c r="G62">
-        <v>0.0007522937014116734</v>
+        <v>-0.001926431546492438</v>
       </c>
       <c r="H62">
-        <v>29.55968424833608</v>
+        <v>29.54892875678961</v>
       </c>
       <c r="I62">
-        <v>34.12833818153045</v>
+        <v>34.12664753478998</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -1476,28 +1476,28 @@
         <v>56</v>
       </c>
       <c r="B63">
-        <v>2009.81528168955</v>
+        <v>2009.911759163232</v>
       </c>
       <c r="C63">
-        <v>602.9445885376979</v>
+        <v>602.9735305280847</v>
       </c>
       <c r="D63">
-        <v>59.99987326924993</v>
+        <v>59.99831629691234</v>
       </c>
       <c r="E63">
-        <v>60.00021625807812</v>
+        <v>59.9985584158129</v>
       </c>
       <c r="F63">
-        <v>-0.004836555941451451</v>
+        <v>-0.004668075256308243</v>
       </c>
       <c r="G63">
-        <v>-0.001124051604098369</v>
+        <v>0.0009960316073326252</v>
       </c>
       <c r="H63">
-        <v>17.23624520930266</v>
+        <v>17.23487101640739</v>
       </c>
       <c r="I63">
-        <v>99.51515143735945</v>
+        <v>99.50396450329896</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -1536,28 +1536,28 @@
         <v>58</v>
       </c>
       <c r="B67">
-        <v>1492.664422274971</v>
+        <v>1354.966545725536</v>
       </c>
       <c r="C67">
-        <v>746.3322131690232</v>
+        <v>677.4830753872644</v>
       </c>
       <c r="D67">
-        <v>-30.00020964141612</v>
+        <v>-244.7914401695775</v>
       </c>
       <c r="E67">
-        <v>-30.00009391353698</v>
+        <v>-244.791451197598</v>
       </c>
       <c r="F67">
-        <v>-0.001134635891084315</v>
+        <v>0.000800023647319108</v>
       </c>
       <c r="G67">
-        <v>1.726125258277022E-05</v>
+        <v>0.001738821151774914</v>
       </c>
       <c r="H67">
-        <v>20.0981825890309</v>
+        <v>180.6622819899379</v>
       </c>
       <c r="I67">
-        <v>40.19670076572509</v>
+        <v>361.3242919723191</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -1565,28 +1565,28 @@
         <v>59</v>
       </c>
       <c r="B68">
-        <v>586.4879829573833</v>
+        <v>586.5178881786698</v>
       </c>
       <c r="C68">
-        <v>390.9920572034896</v>
+        <v>391.0120092064996</v>
       </c>
       <c r="D68">
-        <v>49.99969066422425</v>
+        <v>50.00088414298119</v>
       </c>
       <c r="E68">
-        <v>50.0022101445969</v>
+        <v>50.00032187178126</v>
       </c>
       <c r="F68">
-        <v>-0.006257545078988984</v>
+        <v>-0.003077345396932287</v>
       </c>
       <c r="G68">
-        <v>0.000475867418026269</v>
+        <v>0.001435616236097076</v>
       </c>
       <c r="H68">
-        <v>85.25248643040224</v>
+        <v>85.25069180540693</v>
       </c>
       <c r="I68">
-        <v>127.8892547627229</v>
+        <v>127.8807575797848</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -1625,28 +1625,28 @@
         <v>61</v>
       </c>
       <c r="B72">
-        <v>19997.75723962632</v>
+        <v>19998.72825263309</v>
       </c>
       <c r="C72">
-        <v>19981.41654245573</v>
+        <v>19991.83895448359</v>
       </c>
       <c r="D72">
-        <v>582.6315257369653</v>
+        <v>201.5599338450356</v>
       </c>
       <c r="E72">
-        <v>582.1956903674263</v>
+        <v>201.4931175594023</v>
       </c>
       <c r="F72">
-        <v>66.998623982542</v>
+        <v>62.34267563938607</v>
       </c>
       <c r="G72">
-        <v>175.9199282817469</v>
+        <v>171.5737345339758</v>
       </c>
       <c r="H72">
-        <v>16.93186000817659</v>
+        <v>6.090886458193824</v>
       </c>
       <c r="I72">
-        <v>17.57337002406266</v>
+        <v>7.642764277038633</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -1654,28 +1654,28 @@
         <v>62</v>
       </c>
       <c r="B73">
-        <v>19997.75723962632</v>
+        <v>19998.72825263309</v>
       </c>
       <c r="C73">
-        <v>19991.44039087657</v>
+        <v>19992.41183508806</v>
       </c>
       <c r="D73">
-        <v>216.8396807166607</v>
+        <v>216.838315631131</v>
       </c>
       <c r="E73">
-        <v>216.7774766492678</v>
+        <v>216.7761191043386</v>
       </c>
       <c r="F73">
-        <v>4.860091400329917</v>
+        <v>4.849509963305447</v>
       </c>
       <c r="G73">
-        <v>114.0867592606651</v>
+        <v>114.0867981039294</v>
       </c>
       <c r="H73">
-        <v>6.261888108244006</v>
+        <v>6.261562773531336</v>
       </c>
       <c r="I73">
-        <v>7.074625567814897</v>
+        <v>7.074249419303102</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -1683,28 +1683,28 @@
         <v>63</v>
       </c>
       <c r="B74">
-        <v>390.9920215025131</v>
+        <v>391.0119755478833</v>
       </c>
       <c r="C74">
-        <v>390.3614997407959</v>
+        <v>390.3814865225988</v>
       </c>
       <c r="D74">
-        <v>40.06457288426982</v>
+        <v>40.06456786865245</v>
       </c>
       <c r="E74">
-        <v>39.99999844378982</v>
+        <v>39.99999999999748</v>
       </c>
       <c r="F74">
-        <v>0.05249948831484329</v>
+        <v>0.05249420216037322</v>
       </c>
       <c r="G74">
-        <v>-5.679085609244794E-08</v>
+        <v>1.8712853488978E-12</v>
       </c>
       <c r="H74">
-        <v>59.16057266012713</v>
+        <v>59.15754605399238</v>
       </c>
       <c r="I74">
-        <v>59.16057266012713</v>
+        <v>59.15754605399238</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -1712,28 +1712,28 @@
         <v>64</v>
       </c>
       <c r="B75">
-        <v>19997.75723962632</v>
+        <v>19998.72825263309</v>
       </c>
       <c r="C75">
-        <v>19996.52758431912</v>
+        <v>19997.49870920183</v>
       </c>
       <c r="D75">
-        <v>93.57218479693776</v>
+        <v>93.57035151509126</v>
       </c>
       <c r="E75">
-        <v>93.56437262763318</v>
+        <v>93.56254034252444</v>
       </c>
       <c r="F75">
-        <v>-64.1677747988345</v>
+        <v>-64.17226655444813</v>
       </c>
       <c r="G75">
-        <v>8.691112152841136</v>
+        <v>8.69369758948239</v>
       </c>
       <c r="H75">
-        <v>3.275636477606379</v>
+        <v>3.275554842425507</v>
       </c>
       <c r="I75">
-        <v>2.713100905171892</v>
+        <v>2.712936233227784</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -1741,28 +1741,28 @@
         <v>65</v>
       </c>
       <c r="B76">
-        <v>392.630725570652</v>
+        <v>392.6505533150195</v>
       </c>
       <c r="C76">
-        <v>383.6890695056338</v>
+        <v>383.7093736109052</v>
       </c>
       <c r="D76">
-        <v>204.1258983340154</v>
+        <v>204.1254871459476</v>
       </c>
       <c r="E76">
-        <v>199.9999770326304</v>
+        <v>199.9999999999996</v>
       </c>
       <c r="F76">
-        <v>100.2188166816432</v>
+        <v>100.2184755577707</v>
       </c>
       <c r="G76">
-        <v>96.86440911954156</v>
+        <v>96.86442096756912</v>
       </c>
       <c r="H76">
-        <v>334.3854571290636</v>
+        <v>334.3678018927345</v>
       </c>
       <c r="I76">
-        <v>334.3854571290636</v>
+        <v>334.3678018927345</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -1770,28 +1770,28 @@
         <v>66</v>
       </c>
       <c r="B77">
-        <v>392.630725570652</v>
+        <v>392.6505533150195</v>
       </c>
       <c r="C77">
-        <v>390.6949334566526</v>
+        <v>390.7147973406008</v>
       </c>
       <c r="D77">
-        <v>105.3023662202068</v>
+        <v>105.3013590213881</v>
       </c>
       <c r="E77">
-        <v>104.8396612734503</v>
+        <v>104.8387077912311</v>
       </c>
       <c r="F77">
-        <v>22.57881868669629</v>
+        <v>22.57955097770001</v>
       </c>
       <c r="G77">
-        <v>22.20263580315441</v>
+        <v>22.20341176619027</v>
       </c>
       <c r="H77">
-        <v>158.3698441106598</v>
+        <v>158.3617801789023</v>
       </c>
       <c r="I77">
-        <v>158.3698441106598</v>
+        <v>158.3617801789023</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -1799,28 +1799,28 @@
         <v>67</v>
       </c>
       <c r="B78">
-        <v>2009.81528168955</v>
+        <v>2009.911759163232</v>
       </c>
       <c r="C78">
-        <v>2029.411106824899</v>
+        <v>2029.50666434999</v>
       </c>
       <c r="D78">
-        <v>-278.0358415195804</v>
+        <v>-278.0360268661007</v>
       </c>
       <c r="E78">
-        <v>-279.9999994790002</v>
+        <v>-280.0000000000017</v>
       </c>
       <c r="F78">
-        <v>-167.278856110206</v>
+        <v>-167.2791613907123</v>
       </c>
       <c r="G78">
-        <v>-169.7727224533312</v>
+        <v>-169.7727227629073</v>
       </c>
       <c r="H78">
-        <v>93.21135910512457</v>
+        <v>93.20697572347362</v>
       </c>
       <c r="I78">
-        <v>93.15643607982241</v>
+        <v>93.15205006387311</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -1859,28 +1859,28 @@
         <v>69</v>
       </c>
       <c r="B82">
-        <v>586.0423178039709</v>
+        <v>586.0722512124808</v>
       </c>
       <c r="C82">
-        <v>586.4879829573833</v>
+        <v>586.5178881786698</v>
       </c>
       <c r="D82">
-        <v>-65.16277787202941</v>
+        <v>-65.16158679284047</v>
       </c>
       <c r="E82">
-        <v>-65.21141776491942</v>
+        <v>-65.21022090988882</v>
       </c>
       <c r="F82">
-        <v>-50.44338323266573</v>
+        <v>-50.44377331627581</v>
       </c>
       <c r="G82">
-        <v>-50.4829205184717</v>
+        <v>-50.4833059055368</v>
       </c>
       <c r="H82">
-        <v>140.6096317784082</v>
+        <v>140.60076817509</v>
       </c>
       <c r="I82">
-        <v>140.609624112097</v>
+        <v>140.6007605085263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>